<commit_message>
added directions for use and changed num companies for submission
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack\Desktop\folders\uni\Year 4\Sem 2\SOFTENG 762\group assignment\rpa bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E662CB3-E619-4459-9D74-98FBC6B0D250}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E05E20A-FD40-466C-B464-4FAE9A45BE9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6180" yWindow="3960" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +478,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>

</xml_diff>